<commit_message>
Update test spreadsheet files
</commit_message>
<xml_diff>
--- a/inst/extdata/input_files/test3.xlsx
+++ b/inst/extdata/input_files/test3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowde002\Documents\RTQ_analysis\inst\extdata\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gage1\Documents\Work\quicR\inst\extdata\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0655E7-9B99-4809-81A6-D6515A5CCF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1"/>
+    <workbookView xWindow="7200" yWindow="30" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="83">
   <si>
     <t>User: USER</t>
   </si>
@@ -275,17 +276,11 @@
   <si>
     <t>3. Dilutions</t>
   </si>
-  <si>
-    <t>Tissue</t>
-  </si>
-  <si>
-    <t>LN</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -829,11 +824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49:M56"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,291 +1712,16 @@
       <c r="L45" s="15"/>
       <c r="M45" s="16"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="8">
-        <v>1</v>
-      </c>
-      <c r="C48" s="8">
-        <v>2</v>
-      </c>
-      <c r="D48" s="8">
-        <v>3</v>
-      </c>
-      <c r="E48" s="8">
-        <v>4</v>
-      </c>
-      <c r="F48" s="8">
-        <v>5</v>
-      </c>
-      <c r="G48" s="8">
-        <v>6</v>
-      </c>
-      <c r="H48" s="8">
-        <v>7</v>
-      </c>
-      <c r="I48" s="8">
-        <v>8</v>
-      </c>
-      <c r="J48" s="8">
-        <v>9</v>
-      </c>
-      <c r="K48" s="8">
-        <v>10</v>
-      </c>
-      <c r="L48" s="8">
-        <v>11</v>
-      </c>
-      <c r="M48" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="11"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="13"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="13"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="13"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="13"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="13"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="13"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="16"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AY1" sqref="AY1:BD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>